<commit_message>
Logs for dz2z3.c added.
</commit_message>
<xml_diff>
--- a/MPI/racunanje_ubrzanja_programa_mpi.xlsx
+++ b/MPI/racunanje_ubrzanja_programa_mpi.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saren\OneDrive\Documents\ETF\7. semestar\Multiprocesorski sistemi\GitHub_Domaci\Multiprocessing_Systems\MPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF32B47E-4729-4FD6-AF66-92B0B1F5BABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC619296-9A94-4B02-8924-8375E44C091D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{E700D36A-9AEC-48B1-B431-3A7C21838328}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{E700D36A-9AEC-48B1-B431-3A7C21838328}"/>
   </bookViews>
   <sheets>
-    <sheet name="Zadatak 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Zadatak 1" sheetId="3" r:id="rId1"/>
     <sheet name="Zadatak 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Zadatak 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Zadatak 3" sheetId="1" r:id="rId3"/>
     <sheet name="Zadatak 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -38,9 +38,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="11">
+  <si>
+    <t>sequential</t>
+  </si>
+  <si>
+    <t>30 particles, 100 iterations</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>30 particles, 1000 iterations</t>
+  </si>
+  <si>
+    <t>3000 particles, 100 iterations</t>
+  </si>
+  <si>
+    <t>3000 particles, 1000 iterations</t>
+  </si>
+  <si>
+    <t>speedup</t>
+  </si>
+  <si>
+    <t>parallel (one process)</t>
+  </si>
+  <si>
+    <t>parallel (two processes)</t>
+  </si>
+  <si>
+    <t>parallel (four processes)</t>
+  </si>
+  <si>
+    <t>parallel (eight processes)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,16 +86,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -65,12 +135,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,7 +568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D802E11-FFBF-4034-8D69-C48F8BCDD2DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E507908-E47E-43FA-866F-ABBDC664C0C3}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -408,7 +592,966 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E507908-E47E-43FA-866F-ABBDC664C0C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D802E11-FFBF-4034-8D69-C48F8BCDD2DC}">
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>7.7799999999999996E-3</v>
+      </c>
+      <c r="B3" s="5">
+        <f>AVERAGE(A3:A7)</f>
+        <v>6.4991999999999992E-3</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3.4301999999999999E-2</v>
+      </c>
+      <c r="D3" s="5">
+        <f>AVERAGE(C3:C7)</f>
+        <v>4.93788E-2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2.4107050000000001</v>
+      </c>
+      <c r="F3" s="5">
+        <f>AVERAGE(E3:E7)</f>
+        <v>2.3921540000000001</v>
+      </c>
+      <c r="G3" s="3">
+        <v>23.769746000000001</v>
+      </c>
+      <c r="H3" s="5">
+        <f>AVERAGE(G3:G7)</f>
+        <v>23.8937372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>5.986E-3</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="3">
+        <v>3.2233999999999999E-2</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="3">
+        <v>2.3849840000000002</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="3">
+        <v>23.880281</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>6.3420000000000004E-3</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="3">
+        <v>3.2267999999999998E-2</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="3">
+        <v>2.418174</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="3">
+        <v>23.901166</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>6.0850000000000001E-3</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="3">
+        <v>6.1054999999999998E-2</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="3">
+        <v>2.374854</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="3">
+        <v>23.998033</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6.3029999999999996E-3</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="3">
+        <v>8.7035000000000001E-2</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="3">
+        <v>2.3720530000000002</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="3">
+        <v>23.919460000000001</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>4.3769999999999998E-3</v>
+      </c>
+      <c r="B11" s="9">
+        <f>AVERAGE(A11:A15)</f>
+        <v>4.4596000000000002E-3</v>
+      </c>
+      <c r="C11" s="10">
+        <f>B3/B11</f>
+        <v>1.4573504350165931</v>
+      </c>
+      <c r="D11" s="7">
+        <v>6.8006999999999998E-2</v>
+      </c>
+      <c r="E11" s="9">
+        <f>AVERAGE(D11:D15)</f>
+        <v>6.4985799999999996E-2</v>
+      </c>
+      <c r="F11" s="10">
+        <f>D3/E11</f>
+        <v>0.75983984193469967</v>
+      </c>
+      <c r="G11" s="7">
+        <v>6.6232480000000002</v>
+      </c>
+      <c r="H11" s="9">
+        <f>AVERAGE(G11:G15)</f>
+        <v>6.686429200000001</v>
+      </c>
+      <c r="I11" s="10">
+        <f>F3/H11</f>
+        <v>0.3577625558347346</v>
+      </c>
+      <c r="J11" s="7">
+        <v>89.042483000000004</v>
+      </c>
+      <c r="K11" s="9">
+        <f>AVERAGE(J11:J15)</f>
+        <v>74.137772400000017</v>
+      </c>
+      <c r="L11" s="10">
+        <f>H3/K11</f>
+        <v>0.32228830765354899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>4.4380000000000001E-3</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="7">
+        <v>4.1998000000000001E-2</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="7">
+        <v>6.5891760000000001</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="7">
+        <v>71.662083999999993</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="12"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>4.5110000000000003E-3</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="7">
+        <v>4.3872000000000001E-2</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="7">
+        <v>6.7215730000000002</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="7">
+        <v>69.002851000000007</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="12"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>4.5250000000000004E-3</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="7">
+        <v>5.8254E-2</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="7">
+        <v>6.7527499999999998</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="7">
+        <v>68.275855000000007</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>4.4470000000000004E-3</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="7">
+        <v>0.112798</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="7">
+        <v>6.7453989999999999</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="7">
+        <v>72.705589000000003</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="B19" s="9">
+        <f>AVERAGE(A19:A23)</f>
+        <v>4.6842000000000003E-3</v>
+      </c>
+      <c r="C19" s="10">
+        <f>B3/B19</f>
+        <v>1.3874727808377094</v>
+      </c>
+      <c r="D19" s="7">
+        <v>5.6577000000000002E-2</v>
+      </c>
+      <c r="E19" s="9">
+        <f>AVERAGE(D19:D23)</f>
+        <v>4.8751799999999998E-2</v>
+      </c>
+      <c r="F19" s="10">
+        <f>D3/E19</f>
+        <v>1.0128610635914983</v>
+      </c>
+      <c r="G19" s="7">
+        <v>3.4884689999999998</v>
+      </c>
+      <c r="H19" s="9">
+        <f>AVERAGE(G19:G23)</f>
+        <v>3.6097006</v>
+      </c>
+      <c r="I19" s="10">
+        <f>F3/H19</f>
+        <v>0.6627014993985928</v>
+      </c>
+      <c r="J19" s="7">
+        <v>40.36327</v>
+      </c>
+      <c r="K19" s="9">
+        <f>AVERAGE(J19:J23)</f>
+        <v>41.001088199999991</v>
+      </c>
+      <c r="L19" s="10">
+        <f>H3/K19</f>
+        <v>0.58275861078243296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>4.7720000000000002E-3</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="7">
+        <v>6.0916999999999999E-2</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="7">
+        <v>3.561401</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="7">
+        <v>47.20411</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="12"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>4.9020000000000001E-3</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="7">
+        <v>4.2832000000000002E-2</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="7">
+        <v>3.6326170000000002</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="7">
+        <v>41.847327999999997</v>
+      </c>
+      <c r="K21" s="11"/>
+      <c r="L21" s="12"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>4.4450000000000002E-3</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="7">
+        <v>4.1216999999999997E-2</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="7">
+        <v>3.6529639999999999</v>
+      </c>
+      <c r="H22" s="11"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="7">
+        <v>37.903092999999998</v>
+      </c>
+      <c r="K22" s="11"/>
+      <c r="L22" s="12"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>4.4019999999999997E-3</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="7">
+        <v>4.2215999999999997E-2</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="7">
+        <v>3.7130519999999998</v>
+      </c>
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="7">
+        <v>37.687640000000002</v>
+      </c>
+      <c r="K23" s="13"/>
+      <c r="L23" s="14"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>4.3699999999999998E-3</v>
+      </c>
+      <c r="B27" s="9">
+        <f>AVERAGE(A27:A31)</f>
+        <v>4.3296000000000003E-3</v>
+      </c>
+      <c r="C27" s="10">
+        <f>B3/B27</f>
+        <v>1.5011086474501105</v>
+      </c>
+      <c r="D27" s="7">
+        <v>6.8677000000000002E-2</v>
+      </c>
+      <c r="E27" s="9">
+        <f>AVERAGE(D27:D31)</f>
+        <v>5.2304200000000002E-2</v>
+      </c>
+      <c r="F27" s="10">
+        <f>D3/E27</f>
+        <v>0.94406950111080945</v>
+      </c>
+      <c r="G27" s="7">
+        <v>1.9634100000000001</v>
+      </c>
+      <c r="H27" s="9">
+        <f>AVERAGE(G27:G31)</f>
+        <v>2.189451</v>
+      </c>
+      <c r="I27" s="10">
+        <f>F3/H27</f>
+        <v>1.0925816563147566</v>
+      </c>
+      <c r="J27" s="7">
+        <v>22.983543000000001</v>
+      </c>
+      <c r="K27" s="9">
+        <f>AVERAGE(J27:J31)</f>
+        <v>24.474444599999998</v>
+      </c>
+      <c r="L27" s="10">
+        <f>H3/K27</f>
+        <v>0.97627290794578447</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>4.2700000000000004E-3</v>
+      </c>
+      <c r="B28" s="11"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="7">
+        <v>4.2324000000000001E-2</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="7">
+        <v>2.1728649999999998</v>
+      </c>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="7">
+        <v>23.784718999999999</v>
+      </c>
+      <c r="K28" s="11"/>
+      <c r="L28" s="12"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>4.4650000000000002E-3</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="7">
+        <v>4.3873000000000002E-2</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="7">
+        <v>2.1944849999999998</v>
+      </c>
+      <c r="H29" s="11"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="7">
+        <v>25.523700000000002</v>
+      </c>
+      <c r="K29" s="11"/>
+      <c r="L29" s="12"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>4.3579999999999999E-3</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="7">
+        <v>4.1213E-2</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="7">
+        <v>2.3042750000000001</v>
+      </c>
+      <c r="H30" s="11"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="7">
+        <v>27.042113000000001</v>
+      </c>
+      <c r="K30" s="11"/>
+      <c r="L30" s="12"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>4.1850000000000004E-3</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="7">
+        <v>6.5434000000000006E-2</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="7">
+        <v>2.3122199999999999</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="7">
+        <v>23.038148</v>
+      </c>
+      <c r="K31" s="13"/>
+      <c r="L31" s="14"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L34" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="B35" s="9">
+        <f>AVERAGE(A35:A39)</f>
+        <v>5.8130000000000005E-3</v>
+      </c>
+      <c r="C35" s="10">
+        <f>B3/B35</f>
+        <v>1.1180457595045585</v>
+      </c>
+      <c r="D35" s="7">
+        <v>4.335E-2</v>
+      </c>
+      <c r="E35" s="9">
+        <f>AVERAGE(D35:D39)</f>
+        <v>4.2192600000000004E-2</v>
+      </c>
+      <c r="F35" s="10">
+        <f>D3/E35</f>
+        <v>1.1703189658850128</v>
+      </c>
+      <c r="G35" s="7">
+        <v>1.668833</v>
+      </c>
+      <c r="H35" s="9">
+        <f>AVERAGE(G35:G39)</f>
+        <v>1.9743895999999999</v>
+      </c>
+      <c r="I35" s="10">
+        <f>F3/H35</f>
+        <v>1.2115916737000643</v>
+      </c>
+      <c r="J35" s="7">
+        <v>21.320739</v>
+      </c>
+      <c r="K35" s="9">
+        <f>AVERAGE(J35:J39)</f>
+        <v>21.781726599999999</v>
+      </c>
+      <c r="L35" s="10">
+        <f>H3/K35</f>
+        <v>1.0969624969950731</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>4.5840000000000004E-3</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="7">
+        <v>4.1674000000000003E-2</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="7">
+        <v>2.009665</v>
+      </c>
+      <c r="H36" s="11"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="7">
+        <v>21.419577</v>
+      </c>
+      <c r="K36" s="11"/>
+      <c r="L36" s="12"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>7.3130000000000001E-3</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="7">
+        <v>4.2286999999999998E-2</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="7">
+        <v>2.188358</v>
+      </c>
+      <c r="H37" s="11"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="7">
+        <v>21.917483000000001</v>
+      </c>
+      <c r="K37" s="11"/>
+      <c r="L37" s="12"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>4.6990000000000001E-3</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="7">
+        <v>4.1896999999999997E-2</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="7">
+        <v>2.0170970000000001</v>
+      </c>
+      <c r="H38" s="11"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="7">
+        <v>22.68177</v>
+      </c>
+      <c r="K38" s="11"/>
+      <c r="L38" s="12"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>7.8689999999999993E-3</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="7">
+        <v>4.1755E-2</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="7">
+        <v>1.987995</v>
+      </c>
+      <c r="H39" s="13"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="7">
+        <v>21.569064000000001</v>
+      </c>
+      <c r="K39" s="13"/>
+      <c r="L39" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="41">
+    <mergeCell ref="A33:L33"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="C35:C39"/>
+    <mergeCell ref="E35:E39"/>
+    <mergeCell ref="F35:F39"/>
+    <mergeCell ref="H35:H39"/>
+    <mergeCell ref="I35:I39"/>
+    <mergeCell ref="K35:K39"/>
+    <mergeCell ref="L35:L39"/>
+    <mergeCell ref="L19:L23"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="K27:K31"/>
+    <mergeCell ref="L27:L31"/>
+    <mergeCell ref="K11:K15"/>
+    <mergeCell ref="L11:L15"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="E19:E23"/>
+    <mergeCell ref="F19:F23"/>
+    <mergeCell ref="H19:H23"/>
+    <mergeCell ref="I19:I23"/>
+    <mergeCell ref="K19:K23"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="F11:F15"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="H3:H7"/>
+    <mergeCell ref="A9:L9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118925EF-7105-47D2-92E9-828532FD1FFB}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -417,16 +1560,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118925EF-7105-47D2-92E9-828532FD1FFB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>